<commit_message>
Complete scanning of defectlanding page
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4B21505-7EC7-4470-B75B-E81D0B91C8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64C8173B-CBBD-4E99-B5A5-B3A7E4C6994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="67">
   <si>
     <t>Project Name</t>
   </si>
@@ -87,12 +87,6 @@
   </si>
   <si>
     <t>MD-307</t>
-  </si>
-  <si>
-    <t>Mohit Feature</t>
-  </si>
-  <si>
-    <t>MD-315</t>
   </si>
   <si>
     <t>Project</t>
@@ -673,17 +667,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -704,7 +695,7 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -721,21 +712,11 @@
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -757,22 +738,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -780,19 +761,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -812,19 +793,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -832,16 +813,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -868,19 +849,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -888,16 +869,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -920,22 +901,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -943,19 +924,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -980,13 +961,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
-      </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -994,10 +975,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1020,10 +1001,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1031,7 +1012,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1055,10 +1036,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1066,7 +1047,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1089,10 +1070,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1100,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1120,22 +1101,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
       <c r="F1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1143,19 +1124,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
         <v>35</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1178,25 +1159,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
       <c r="G1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1204,22 +1185,22 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1231,9 +1212,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1242,10 +1221,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1273,16 +1252,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1290,13 +1269,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1316,13 +1295,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1330,10 +1309,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1353,19 +1332,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1373,16 +1352,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1402,16 +1381,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1419,13 +1398,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1445,16 +1424,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1462,13 +1441,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1492,10 +1471,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1527,10 +1506,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1538,7 +1517,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1562,10 +1541,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1573,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1597,10 +1576,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1608,7 +1587,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1628,18 +1607,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1662,22 +1641,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1688,16 +1667,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1726,10 +1705,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1740,10 +1719,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1778,7 +1757,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1792,7 +1771,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1829,13 +1808,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1846,7 +1825,7 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1869,7 +1848,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -1898,10 +1877,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1909,7 +1888,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1921,7 +1900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98E6EE4-5435-41BC-8AD6-B776B53E8FC7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1934,16 +1913,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1954,10 +1933,10 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1981,37 +1960,37 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added TC048->data->method and locator->epicArrowRight,epicArrowDown and methods->clickEpicDropdown
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64C8173B-CBBD-4E99-B5A5-B3A7E4C6994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B41933-8941-472D-9395-07EE088223FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -16,51 +21,41 @@
     <sheet name="tc005" sheetId="3" r:id="rId6"/>
     <sheet name="tc006" sheetId="4" r:id="rId7"/>
     <sheet name="tc029" sheetId="27" r:id="rId8"/>
-    <sheet name="tc007" sheetId="5" r:id="rId9"/>
-    <sheet name="tc008" sheetId="8" r:id="rId10"/>
-    <sheet name="tc009" sheetId="9" r:id="rId11"/>
-    <sheet name="tc011" sheetId="6" r:id="rId12"/>
-    <sheet name="tc021" sheetId="17" r:id="rId13"/>
-    <sheet name="tc022" sheetId="18" r:id="rId14"/>
-    <sheet name="tc036" sheetId="30" r:id="rId15"/>
-    <sheet name="tc035" sheetId="24" r:id="rId16"/>
-    <sheet name="tc037" sheetId="25" r:id="rId17"/>
-    <sheet name="tc027" sheetId="28" r:id="rId18"/>
-    <sheet name="tc024" sheetId="29" r:id="rId19"/>
-    <sheet name="tc010" sheetId="10" r:id="rId20"/>
-    <sheet name="tc017" sheetId="15" r:id="rId21"/>
-    <sheet name="tc018" sheetId="16" r:id="rId22"/>
-    <sheet name="tc030" sheetId="19" r:id="rId23"/>
-    <sheet name="tc026" sheetId="20" r:id="rId24"/>
-    <sheet name="tc015" sheetId="11" r:id="rId25"/>
-    <sheet name="tc025" sheetId="14" r:id="rId26"/>
-    <sheet name="tc032" sheetId="21" r:id="rId27"/>
-    <sheet name="tc033" sheetId="22" r:id="rId28"/>
-    <sheet name="tc004" sheetId="13" r:id="rId29"/>
-    <sheet name="tc019" sheetId="12" r:id="rId30"/>
+    <sheet name="tc048" sheetId="31" r:id="rId9"/>
+    <sheet name="tc007" sheetId="5" r:id="rId10"/>
+    <sheet name="tc008" sheetId="8" r:id="rId11"/>
+    <sheet name="tc009" sheetId="9" r:id="rId12"/>
+    <sheet name="tc011" sheetId="6" r:id="rId13"/>
+    <sheet name="tc021" sheetId="17" r:id="rId14"/>
+    <sheet name="tc022" sheetId="18" r:id="rId15"/>
+    <sheet name="tc036" sheetId="30" r:id="rId16"/>
+    <sheet name="tc035" sheetId="24" r:id="rId17"/>
+    <sheet name="tc037" sheetId="25" r:id="rId18"/>
+    <sheet name="tc027" sheetId="28" r:id="rId19"/>
+    <sheet name="tc024" sheetId="29" r:id="rId20"/>
+    <sheet name="tc010" sheetId="10" r:id="rId21"/>
+    <sheet name="tc017" sheetId="15" r:id="rId22"/>
+    <sheet name="tc018" sheetId="16" r:id="rId23"/>
+    <sheet name="tc030" sheetId="19" r:id="rId24"/>
+    <sheet name="tc026" sheetId="20" r:id="rId25"/>
+    <sheet name="tc015" sheetId="11" r:id="rId26"/>
+    <sheet name="tc025" sheetId="14" r:id="rId27"/>
+    <sheet name="tc032" sheetId="21" r:id="rId28"/>
+    <sheet name="tc033" sheetId="22" r:id="rId29"/>
+    <sheet name="tc004" sheetId="13" r:id="rId30"/>
+    <sheet name="tc019" sheetId="12" r:id="rId31"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="71">
   <si>
     <t>Project Name</t>
   </si>
@@ -261,6 +256,18 @@
   </si>
   <si>
     <t>Mayukhjit Chakraborty</t>
+  </si>
+  <si>
+    <t>ModuleName</t>
+  </si>
+  <si>
+    <t>ReqId</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>Mohit Aman</t>
   </si>
 </sst>
 </file>
@@ -671,13 +678,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="50.453125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -711,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -724,6 +731,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDC4E0-08CB-46D1-AE6D-9F161D97ECBA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -731,9 +791,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -781,7 +841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -789,7 +849,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
@@ -830,7 +890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E68E9-6114-4137-93A6-9E3D35854EF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -838,16 +898,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.1796875" customWidth="1"/>
+    <col min="5" max="5" width="23.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -864,7 +924,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -886,7 +946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C081D6-A9C0-44C4-B61F-ECF5E1994215}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -894,9 +954,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="26.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -944,7 +1004,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339B4C-E482-471A-B298-7F44E9BDAA0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -952,11 +1012,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -986,7 +1046,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -994,12 +1054,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1007,7 +1067,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1020,7 +1080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E83F4D4-5FFA-485C-BDFA-643C5CC60A7E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1028,9 +1088,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1055,7 +1115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC98DF-CF4C-4978-974B-D4FADFCADB14}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1063,9 +1123,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.85546875" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultColWidth="16.81640625" defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1089,7 +1149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A20FB-0778-47B6-A652-A1B2BA52FD0E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1097,7 +1157,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1144,7 +1204,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B902D842-DC6C-4B26-A4EA-6A91C104A4CF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1152,9 +1244,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -1208,39 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AE5E9-3E74-406A-B22D-ED31893F34EB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1248,7 +1308,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
@@ -1283,7 +1343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1291,7 +1351,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
@@ -1320,7 +1380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C944F0C-FA76-4DBA-99AE-F54BD5BF8527}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1328,7 +1388,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
@@ -1369,7 +1429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29E5669-D6FB-40EE-905B-49DC274A1C27}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1377,7 +1437,50 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
@@ -1389,8 +1492,8 @@
       <c r="C1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1401,49 +1504,6 @@
         <v>23</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1455,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE5E322-70B6-4F63-AE80-0840E4095282}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1463,10 +1523,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1490,7 +1550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28779ED8-A79D-4E0B-852B-088D1DC08811}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1498,10 +1558,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="30.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1525,7 +1585,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AFD247-EFEB-43D1-A5E4-94260D9F042E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1533,10 +1593,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="37.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1560,7 +1620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1568,10 +1628,10 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1595,7 +1655,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1603,7 +1721,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1626,65 +1744,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1692,12 +1752,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1711,7 +1771,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1738,15 +1798,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="35.1796875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
+    <col min="3" max="3" width="32.54296875" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1760,7 +1820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1774,7 +1834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1799,11 +1859,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39.54296875" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1841,12 +1901,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1869,13 +1929,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="32.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="32.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1883,7 +1943,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1900,18 +1960,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98E6EE4-5435-41BC-8AD6-B776B53E8FC7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
+    <col min="2" max="2" width="17.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -1925,7 +1985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1945,51 +2005,39 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0C63D3-0E30-4064-90E5-1BC4EA13CB24}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="3" max="3" width="14.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TC049 and data
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B41933-8941-472D-9395-07EE088223FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1D5766-7BE6-442F-96A8-040581E00088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -22,28 +22,29 @@
     <sheet name="tc006" sheetId="4" r:id="rId7"/>
     <sheet name="tc029" sheetId="27" r:id="rId8"/>
     <sheet name="tc048" sheetId="31" r:id="rId9"/>
-    <sheet name="tc007" sheetId="5" r:id="rId10"/>
-    <sheet name="tc008" sheetId="8" r:id="rId11"/>
-    <sheet name="tc009" sheetId="9" r:id="rId12"/>
-    <sheet name="tc011" sheetId="6" r:id="rId13"/>
-    <sheet name="tc021" sheetId="17" r:id="rId14"/>
-    <sheet name="tc022" sheetId="18" r:id="rId15"/>
-    <sheet name="tc036" sheetId="30" r:id="rId16"/>
-    <sheet name="tc035" sheetId="24" r:id="rId17"/>
-    <sheet name="tc037" sheetId="25" r:id="rId18"/>
-    <sheet name="tc027" sheetId="28" r:id="rId19"/>
-    <sheet name="tc024" sheetId="29" r:id="rId20"/>
-    <sheet name="tc010" sheetId="10" r:id="rId21"/>
-    <sheet name="tc017" sheetId="15" r:id="rId22"/>
-    <sheet name="tc018" sheetId="16" r:id="rId23"/>
-    <sheet name="tc030" sheetId="19" r:id="rId24"/>
-    <sheet name="tc026" sheetId="20" r:id="rId25"/>
-    <sheet name="tc015" sheetId="11" r:id="rId26"/>
-    <sheet name="tc025" sheetId="14" r:id="rId27"/>
-    <sheet name="tc032" sheetId="21" r:id="rId28"/>
-    <sheet name="tc033" sheetId="22" r:id="rId29"/>
-    <sheet name="tc004" sheetId="13" r:id="rId30"/>
-    <sheet name="tc019" sheetId="12" r:id="rId31"/>
+    <sheet name="tc049" sheetId="32" r:id="rId10"/>
+    <sheet name="tc007" sheetId="5" r:id="rId11"/>
+    <sheet name="tc008" sheetId="8" r:id="rId12"/>
+    <sheet name="tc009" sheetId="9" r:id="rId13"/>
+    <sheet name="tc011" sheetId="6" r:id="rId14"/>
+    <sheet name="tc021" sheetId="17" r:id="rId15"/>
+    <sheet name="tc022" sheetId="18" r:id="rId16"/>
+    <sheet name="tc036" sheetId="30" r:id="rId17"/>
+    <sheet name="tc035" sheetId="24" r:id="rId18"/>
+    <sheet name="tc037" sheetId="25" r:id="rId19"/>
+    <sheet name="tc027" sheetId="28" r:id="rId20"/>
+    <sheet name="tc024" sheetId="29" r:id="rId21"/>
+    <sheet name="tc010" sheetId="10" r:id="rId22"/>
+    <sheet name="tc017" sheetId="15" r:id="rId23"/>
+    <sheet name="tc018" sheetId="16" r:id="rId24"/>
+    <sheet name="tc030" sheetId="19" r:id="rId25"/>
+    <sheet name="tc026" sheetId="20" r:id="rId26"/>
+    <sheet name="tc015" sheetId="11" r:id="rId27"/>
+    <sheet name="tc025" sheetId="14" r:id="rId28"/>
+    <sheet name="tc032" sheetId="21" r:id="rId29"/>
+    <sheet name="tc033" sheetId="22" r:id="rId30"/>
+    <sheet name="tc004" sheetId="13" r:id="rId31"/>
+    <sheet name="tc019" sheetId="12" r:id="rId32"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="72">
   <si>
     <t>Project Name</t>
   </si>
@@ -268,6 +269,9 @@
   </si>
   <si>
     <t>Mohit Aman</t>
+  </si>
+  <si>
+    <t>Manual</t>
   </si>
 </sst>
 </file>
@@ -731,6 +735,43 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E39B07E-A6B4-481A-B0E9-99CE6DD1014B}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -783,7 +824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDC4E0-08CB-46D1-AE6D-9F161D97ECBA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -841,7 +882,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -890,7 +931,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E68E9-6114-4137-93A6-9E3D35854EF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -946,7 +987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C081D6-A9C0-44C4-B61F-ECF5E1994215}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1004,7 +1045,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339B4C-E482-471A-B298-7F44E9BDAA0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1046,7 +1087,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1080,7 +1121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E83F4D4-5FFA-485C-BDFA-643C5CC60A7E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1115,7 +1156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC98DF-CF4C-4978-974B-D4FADFCADB14}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1149,7 +1190,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A20FB-0778-47B6-A652-A1B2BA52FD0E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1204,39 +1277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B902D842-DC6C-4B26-A4EA-6A91C104A4CF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1300,7 +1341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AE5E9-3E74-406A-B22D-ED31893F34EB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1343,7 +1384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1380,7 +1421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C944F0C-FA76-4DBA-99AE-F54BD5BF8527}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1429,7 +1470,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29E5669-D6FB-40EE-905B-49DC274A1C27}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1472,7 +1513,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1515,7 +1556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE5E322-70B6-4F63-AE80-0840E4095282}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1550,7 +1591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28779ED8-A79D-4E0B-852B-088D1DC08811}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1585,7 +1626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AFD247-EFEB-43D1-A5E4-94260D9F042E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1620,7 +1661,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1655,65 +1754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1744,7 +1785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2008,8 +2049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0C63D3-0E30-4064-90E5-1BC4EA13CB24}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
Added TC050 and data also change the xpath of the AddTestcasePage save button
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1D5766-7BE6-442F-96A8-040581E00088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB44DA7-9873-47C9-A0F9-0DA56A3FEB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -23,28 +23,29 @@
     <sheet name="tc029" sheetId="27" r:id="rId8"/>
     <sheet name="tc048" sheetId="31" r:id="rId9"/>
     <sheet name="tc049" sheetId="32" r:id="rId10"/>
-    <sheet name="tc007" sheetId="5" r:id="rId11"/>
-    <sheet name="tc008" sheetId="8" r:id="rId12"/>
-    <sheet name="tc009" sheetId="9" r:id="rId13"/>
-    <sheet name="tc011" sheetId="6" r:id="rId14"/>
-    <sheet name="tc021" sheetId="17" r:id="rId15"/>
-    <sheet name="tc022" sheetId="18" r:id="rId16"/>
-    <sheet name="tc036" sheetId="30" r:id="rId17"/>
-    <sheet name="tc035" sheetId="24" r:id="rId18"/>
-    <sheet name="tc037" sheetId="25" r:id="rId19"/>
-    <sheet name="tc027" sheetId="28" r:id="rId20"/>
-    <sheet name="tc024" sheetId="29" r:id="rId21"/>
-    <sheet name="tc010" sheetId="10" r:id="rId22"/>
-    <sheet name="tc017" sheetId="15" r:id="rId23"/>
-    <sheet name="tc018" sheetId="16" r:id="rId24"/>
-    <sheet name="tc030" sheetId="19" r:id="rId25"/>
-    <sheet name="tc026" sheetId="20" r:id="rId26"/>
-    <sheet name="tc015" sheetId="11" r:id="rId27"/>
-    <sheet name="tc025" sheetId="14" r:id="rId28"/>
-    <sheet name="tc032" sheetId="21" r:id="rId29"/>
-    <sheet name="tc033" sheetId="22" r:id="rId30"/>
-    <sheet name="tc004" sheetId="13" r:id="rId31"/>
-    <sheet name="tc019" sheetId="12" r:id="rId32"/>
+    <sheet name="tc050" sheetId="33" r:id="rId11"/>
+    <sheet name="tc007" sheetId="5" r:id="rId12"/>
+    <sheet name="tc008" sheetId="8" r:id="rId13"/>
+    <sheet name="tc009" sheetId="9" r:id="rId14"/>
+    <sheet name="tc011" sheetId="6" r:id="rId15"/>
+    <sheet name="tc021" sheetId="17" r:id="rId16"/>
+    <sheet name="tc022" sheetId="18" r:id="rId17"/>
+    <sheet name="tc036" sheetId="30" r:id="rId18"/>
+    <sheet name="tc035" sheetId="24" r:id="rId19"/>
+    <sheet name="tc037" sheetId="25" r:id="rId20"/>
+    <sheet name="tc027" sheetId="28" r:id="rId21"/>
+    <sheet name="tc024" sheetId="29" r:id="rId22"/>
+    <sheet name="tc010" sheetId="10" r:id="rId23"/>
+    <sheet name="tc017" sheetId="15" r:id="rId24"/>
+    <sheet name="tc018" sheetId="16" r:id="rId25"/>
+    <sheet name="tc030" sheetId="19" r:id="rId26"/>
+    <sheet name="tc026" sheetId="20" r:id="rId27"/>
+    <sheet name="tc015" sheetId="11" r:id="rId28"/>
+    <sheet name="tc025" sheetId="14" r:id="rId29"/>
+    <sheet name="tc032" sheetId="21" r:id="rId30"/>
+    <sheet name="tc033" sheetId="22" r:id="rId31"/>
+    <sheet name="tc004" sheetId="13" r:id="rId32"/>
+    <sheet name="tc019" sheetId="12" r:id="rId33"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="74">
   <si>
     <t>Project Name</t>
   </si>
@@ -272,6 +273,12 @@
   </si>
   <si>
     <t>Manual</t>
+  </si>
+  <si>
+    <t>Tcname</t>
+  </si>
+  <si>
+    <t>Unit testing Dec 2025</t>
   </si>
 </sst>
 </file>
@@ -738,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E39B07E-A6B4-481A-B0E9-99CE6DD1014B}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -772,6 +779,52 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF10A50-BF88-4028-B726-1730182C1503}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -824,7 +877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDC4E0-08CB-46D1-AE6D-9F161D97ECBA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -882,7 +935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -931,7 +984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E68E9-6114-4137-93A6-9E3D35854EF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -987,7 +1040,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C081D6-A9C0-44C4-B61F-ECF5E1994215}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1045,7 +1098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339B4C-E482-471A-B298-7F44E9BDAA0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1087,7 +1140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1121,7 +1174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E83F4D4-5FFA-485C-BDFA-643C5CC60A7E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1156,7 +1209,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC98DF-CF4C-4978-974B-D4FADFCADB14}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1190,39 +1275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A20FB-0778-47B6-A652-A1B2BA52FD0E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1277,7 +1330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B902D842-DC6C-4B26-A4EA-6A91C104A4CF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1341,7 +1394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AE5E9-3E74-406A-B22D-ED31893F34EB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1384,7 +1437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1421,7 +1474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C944F0C-FA76-4DBA-99AE-F54BD5BF8527}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1470,7 +1523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29E5669-D6FB-40EE-905B-49DC274A1C27}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1513,7 +1566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1556,7 +1609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE5E322-70B6-4F63-AE80-0840E4095282}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1591,7 +1644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28779ED8-A79D-4E0B-852B-088D1DC08811}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1626,7 +1679,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AFD247-EFEB-43D1-A5E4-94260D9F042E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1661,65 +1772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1754,7 +1807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1785,7 +1838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added TC051 and data
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349A8E80-A8F4-43B6-BA02-94824373CA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2B75FF-84AB-43DA-83B7-539BDB0E3AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -24,28 +24,29 @@
     <sheet name="tc048" sheetId="31" r:id="rId9"/>
     <sheet name="tc049" sheetId="32" r:id="rId10"/>
     <sheet name="tc050" sheetId="33" r:id="rId11"/>
-    <sheet name="tc007" sheetId="5" r:id="rId12"/>
-    <sheet name="tc008" sheetId="8" r:id="rId13"/>
-    <sheet name="tc009" sheetId="9" r:id="rId14"/>
-    <sheet name="tc011" sheetId="6" r:id="rId15"/>
-    <sheet name="tc021" sheetId="17" r:id="rId16"/>
-    <sheet name="tc022" sheetId="18" r:id="rId17"/>
-    <sheet name="tc036" sheetId="30" r:id="rId18"/>
-    <sheet name="tc035" sheetId="24" r:id="rId19"/>
-    <sheet name="tc037" sheetId="25" r:id="rId20"/>
-    <sheet name="tc027" sheetId="28" r:id="rId21"/>
-    <sheet name="tc024" sheetId="29" r:id="rId22"/>
-    <sheet name="tc010" sheetId="10" r:id="rId23"/>
-    <sheet name="tc017" sheetId="15" r:id="rId24"/>
-    <sheet name="tc018" sheetId="16" r:id="rId25"/>
-    <sheet name="tc030" sheetId="19" r:id="rId26"/>
-    <sheet name="tc026" sheetId="20" r:id="rId27"/>
-    <sheet name="tc015" sheetId="11" r:id="rId28"/>
-    <sheet name="tc025" sheetId="14" r:id="rId29"/>
-    <sheet name="tc032" sheetId="21" r:id="rId30"/>
-    <sheet name="tc033" sheetId="22" r:id="rId31"/>
-    <sheet name="tc004" sheetId="13" r:id="rId32"/>
-    <sheet name="tc019" sheetId="12" r:id="rId33"/>
+    <sheet name="tc051" sheetId="34" r:id="rId12"/>
+    <sheet name="tc007" sheetId="5" r:id="rId13"/>
+    <sheet name="tc008" sheetId="8" r:id="rId14"/>
+    <sheet name="tc009" sheetId="9" r:id="rId15"/>
+    <sheet name="tc011" sheetId="6" r:id="rId16"/>
+    <sheet name="tc021" sheetId="17" r:id="rId17"/>
+    <sheet name="tc022" sheetId="18" r:id="rId18"/>
+    <sheet name="tc036" sheetId="30" r:id="rId19"/>
+    <sheet name="tc035" sheetId="24" r:id="rId20"/>
+    <sheet name="tc037" sheetId="25" r:id="rId21"/>
+    <sheet name="tc027" sheetId="28" r:id="rId22"/>
+    <sheet name="tc024" sheetId="29" r:id="rId23"/>
+    <sheet name="tc010" sheetId="10" r:id="rId24"/>
+    <sheet name="tc017" sheetId="15" r:id="rId25"/>
+    <sheet name="tc018" sheetId="16" r:id="rId26"/>
+    <sheet name="tc030" sheetId="19" r:id="rId27"/>
+    <sheet name="tc026" sheetId="20" r:id="rId28"/>
+    <sheet name="tc015" sheetId="11" r:id="rId29"/>
+    <sheet name="tc025" sheetId="14" r:id="rId30"/>
+    <sheet name="tc032" sheetId="21" r:id="rId31"/>
+    <sheet name="tc033" sheetId="22" r:id="rId32"/>
+    <sheet name="tc004" sheetId="13" r:id="rId33"/>
+    <sheet name="tc019" sheetId="12" r:id="rId34"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
   <si>
     <t>Project Name</t>
   </si>
@@ -782,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF10A50-BF88-4028-B726-1730182C1503}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -825,6 +826,37 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EDAF2F-6C72-47C6-8B27-A92EFCB68371}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -877,7 +909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDC4E0-08CB-46D1-AE6D-9F161D97ECBA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -935,7 +967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -984,7 +1016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E68E9-6114-4137-93A6-9E3D35854EF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1040,7 +1072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C081D6-A9C0-44C4-B61F-ECF5E1994215}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1098,7 +1130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339B4C-E482-471A-B298-7F44E9BDAA0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1140,7 +1172,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1174,7 +1206,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E83F4D4-5FFA-485C-BDFA-643C5CC60A7E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1209,39 +1273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC98DF-CF4C-4978-974B-D4FADFCADB14}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1275,7 +1307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A20FB-0778-47B6-A652-A1B2BA52FD0E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1330,7 +1362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B902D842-DC6C-4B26-A4EA-6A91C104A4CF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1394,7 +1426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AE5E9-3E74-406A-B22D-ED31893F34EB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1437,7 +1469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1474,7 +1506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C944F0C-FA76-4DBA-99AE-F54BD5BF8527}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1523,7 +1555,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29E5669-D6FB-40EE-905B-49DC274A1C27}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1566,7 +1598,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1609,7 +1641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE5E322-70B6-4F63-AE80-0840E4095282}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1644,7 +1676,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28779ED8-A79D-4E0B-852B-088D1DC08811}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1679,65 +1769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AFD247-EFEB-43D1-A5E4-94260D9F042E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1772,7 +1804,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1807,7 +1839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1838,7 +1870,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added TC-74 		addedtestcase: modified settestcasename
Added TC-75
		AuthorTestcasePage: added opentestcasebyid
		IndividualTestcasePage: Modified method for the priority

Added TC-76

added data provider for TC74,75,76
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A159337-BD38-475A-842A-86BC743119F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191748A3-B13E-4464-8674-B1BBC2F95CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -25,28 +25,29 @@
     <sheet name="tc049" sheetId="32" r:id="rId10"/>
     <sheet name="tc050" sheetId="33" r:id="rId11"/>
     <sheet name="tc051" sheetId="34" r:id="rId12"/>
-    <sheet name="tc007" sheetId="5" r:id="rId13"/>
-    <sheet name="tc008" sheetId="8" r:id="rId14"/>
-    <sheet name="tc009" sheetId="9" r:id="rId15"/>
-    <sheet name="tc011" sheetId="6" r:id="rId16"/>
-    <sheet name="tc021" sheetId="17" r:id="rId17"/>
-    <sheet name="tc022" sheetId="18" r:id="rId18"/>
-    <sheet name="tc036" sheetId="30" r:id="rId19"/>
-    <sheet name="tc035" sheetId="24" r:id="rId20"/>
-    <sheet name="tc037" sheetId="25" r:id="rId21"/>
-    <sheet name="tc027" sheetId="28" r:id="rId22"/>
-    <sheet name="tc024" sheetId="29" r:id="rId23"/>
-    <sheet name="tc010" sheetId="10" r:id="rId24"/>
-    <sheet name="tc017" sheetId="15" r:id="rId25"/>
-    <sheet name="tc018" sheetId="16" r:id="rId26"/>
-    <sheet name="tc030" sheetId="19" r:id="rId27"/>
-    <sheet name="tc026" sheetId="20" r:id="rId28"/>
-    <sheet name="tc015" sheetId="11" r:id="rId29"/>
-    <sheet name="tc025" sheetId="14" r:id="rId30"/>
-    <sheet name="tc032" sheetId="21" r:id="rId31"/>
-    <sheet name="tc033" sheetId="22" r:id="rId32"/>
-    <sheet name="tc004" sheetId="13" r:id="rId33"/>
-    <sheet name="tc019" sheetId="12" r:id="rId34"/>
+    <sheet name="tc074" sheetId="35" r:id="rId13"/>
+    <sheet name="tc007" sheetId="5" r:id="rId14"/>
+    <sheet name="tc008" sheetId="8" r:id="rId15"/>
+    <sheet name="tc009" sheetId="9" r:id="rId16"/>
+    <sheet name="tc011" sheetId="6" r:id="rId17"/>
+    <sheet name="tc021" sheetId="17" r:id="rId18"/>
+    <sheet name="tc022" sheetId="18" r:id="rId19"/>
+    <sheet name="tc036" sheetId="30" r:id="rId20"/>
+    <sheet name="tc035" sheetId="24" r:id="rId21"/>
+    <sheet name="tc037" sheetId="25" r:id="rId22"/>
+    <sheet name="tc027" sheetId="28" r:id="rId23"/>
+    <sheet name="tc024" sheetId="29" r:id="rId24"/>
+    <sheet name="tc010" sheetId="10" r:id="rId25"/>
+    <sheet name="tc017" sheetId="15" r:id="rId26"/>
+    <sheet name="tc018" sheetId="16" r:id="rId27"/>
+    <sheet name="tc030" sheetId="19" r:id="rId28"/>
+    <sheet name="tc026" sheetId="20" r:id="rId29"/>
+    <sheet name="tc015" sheetId="11" r:id="rId30"/>
+    <sheet name="tc025" sheetId="14" r:id="rId31"/>
+    <sheet name="tc032" sheetId="21" r:id="rId32"/>
+    <sheet name="tc033" sheetId="22" r:id="rId33"/>
+    <sheet name="tc004" sheetId="13" r:id="rId34"/>
+    <sheet name="tc019" sheetId="12" r:id="rId35"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="78">
   <si>
     <t>Project Name</t>
   </si>
@@ -280,6 +281,18 @@
   </si>
   <si>
     <t>Unit testing Dec 2025</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Mohit Feature</t>
+  </si>
+  <si>
+    <t>RQ-489</t>
   </si>
 </sst>
 </file>
@@ -829,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EDAF2F-6C72-47C6-8B27-A92EFCB68371}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
@@ -857,6 +870,43 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E05E90-869C-4175-A1A5-AEBD769E7397}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -909,7 +959,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DDC4E0-08CB-46D1-AE6D-9F161D97ECBA}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -967,7 +1017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1016,7 +1066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E68E9-6114-4137-93A6-9E3D35854EF2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1072,7 +1122,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C081D6-A9C0-44C4-B61F-ECF5E1994215}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1130,7 +1180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1339B4C-E482-471A-B298-7F44E9BDAA0D}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1172,7 +1222,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1206,39 +1288,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{710D6ACC-846B-479B-9D45-4664C5AACF8A}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E83F4D4-5FFA-485C-BDFA-643C5CC60A7E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1273,7 +1323,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FC98DF-CF4C-4978-974B-D4FADFCADB14}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1307,7 +1357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816A20FB-0778-47B6-A652-A1B2BA52FD0E}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1362,7 +1412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B902D842-DC6C-4B26-A4EA-6A91C104A4CF}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1426,7 +1476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657AE5E9-3E74-406A-B22D-ED31893F34EB}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1469,7 +1519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1506,7 +1556,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C944F0C-FA76-4DBA-99AE-F54BD5BF8527}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -1555,7 +1605,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29E5669-D6FB-40EE-905B-49DC274A1C27}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1598,7 +1648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AF5BF0-3AF2-4AD0-B35F-8942D3128B73}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1641,7 +1691,65 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE5E322-70B6-4F63-AE80-0840E4095282}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1676,65 +1784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEF2594-B7B7-40EF-9BFC-A865F0ACD5B2}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="39" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28779ED8-A79D-4E0B-852B-088D1DC08811}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1769,7 +1819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3AFD247-EFEB-43D1-A5E4-94260D9F042E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1804,7 +1854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1839,7 +1889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1870,7 +1920,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TC-64 added and method:verifyRequirementUpdateNotification in RequirementTabPage.java, added data for TC-64
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C529710-C5CD-4232-9D7D-D82B858D4F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B488428-3CC7-449E-909C-2CCF76D290D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="43" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="44" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,11 @@
     <sheet name="tc054" sheetId="46" r:id="rId42"/>
     <sheet name="tc055" sheetId="47" r:id="rId43"/>
     <sheet name="tc063" sheetId="48" r:id="rId44"/>
-    <sheet name="tc047" sheetId="37" r:id="rId45"/>
-    <sheet name="tc046" sheetId="38" r:id="rId46"/>
-    <sheet name="tc004" sheetId="13" r:id="rId47"/>
-    <sheet name="tc019" sheetId="12" r:id="rId48"/>
+    <sheet name="tc064" sheetId="49" r:id="rId45"/>
+    <sheet name="tc047" sheetId="37" r:id="rId46"/>
+    <sheet name="tc046" sheetId="38" r:id="rId47"/>
+    <sheet name="tc004" sheetId="13" r:id="rId48"/>
+    <sheet name="tc019" sheetId="12" r:id="rId49"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="95">
   <si>
     <t>Project Name</t>
   </si>
@@ -2511,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1567252D-CB85-4108-A7F9-F9A0823679CB}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2568,6 +2569,67 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA50CB24-998A-4723-A6C2-7AE3CF313CCB}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294C6248-6B39-4869-9A5F-1A9888AB4466}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2610,7 +2672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5D97A-4287-4435-9AB2-0BB45EA4FBC3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2647,7 +2709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2678,7 +2740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TC-73 added in requirement tab
added method DeleteRequirementById(String rqId) in RequirementTabPage

added data for TC073
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FFF851-97D4-40FC-8FDF-1D55BD7527AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5E1759-C6AD-4E0C-93AB-327FD48A4DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="44" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -58,10 +58,11 @@
     <sheet name="tc055" sheetId="47" r:id="rId43"/>
     <sheet name="tc063" sheetId="48" r:id="rId44"/>
     <sheet name="tc064" sheetId="49" r:id="rId45"/>
-    <sheet name="tc047" sheetId="37" r:id="rId46"/>
-    <sheet name="tc046" sheetId="38" r:id="rId47"/>
-    <sheet name="tc004" sheetId="13" r:id="rId48"/>
-    <sheet name="tc019" sheetId="12" r:id="rId49"/>
+    <sheet name="tc073" sheetId="50" r:id="rId46"/>
+    <sheet name="tc047" sheetId="37" r:id="rId47"/>
+    <sheet name="tc046" sheetId="38" r:id="rId48"/>
+    <sheet name="tc004" sheetId="13" r:id="rId49"/>
+    <sheet name="tc019" sheetId="12" r:id="rId50"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="97">
   <si>
     <t>Project Name</t>
   </si>
@@ -358,6 +359,12 @@
   </si>
   <si>
     <t>Flow testing</t>
+  </si>
+  <si>
+    <t>Notification for New Requirement 8-01-2026</t>
+  </si>
+  <si>
+    <t>delete notification Flow testing</t>
   </si>
 </sst>
 </file>
@@ -2572,7 +2579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA50CB24-998A-4723-A6C2-7AE3CF313CCB}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -2630,6 +2637,66 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3E5496-AF76-431E-B66C-9B684F671DD4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="2" width="52.54296875" customWidth="1"/>
+    <col min="3" max="3" width="27.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294C6248-6B39-4869-9A5F-1A9888AB4466}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2672,7 +2739,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5D97A-4287-4435-9AB2-0BB45EA4FBC3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2709,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2740,7 +2807,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BEAA1A-A534-4468-B9EC-E9F8BB732A2D}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="39.54296875" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="16.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2789,48 +2898,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29BEAA1A-A534-4468-B9EC-E9F8BB732A2D}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="39.54296875" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326BFDAD-078A-4AAF-9BA5-44F9F397DA35}">
   <dimension ref="A1:A2"/>

</xml_diff>

<commit_message>
TC-74 added in requirement tab
added method clickEpic(),verifyModuleCreationNotification(String moduleName) in RequirementTabPage

added data for TC074
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5E1759-C6AD-4E0C-93AB-327FD48A4DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F80C95C-7D4E-4393-9143-1A58CE6465D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="45" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -59,10 +59,11 @@
     <sheet name="tc063" sheetId="48" r:id="rId44"/>
     <sheet name="tc064" sheetId="49" r:id="rId45"/>
     <sheet name="tc073" sheetId="50" r:id="rId46"/>
-    <sheet name="tc047" sheetId="37" r:id="rId47"/>
-    <sheet name="tc046" sheetId="38" r:id="rId48"/>
-    <sheet name="tc004" sheetId="13" r:id="rId49"/>
-    <sheet name="tc019" sheetId="12" r:id="rId50"/>
+    <sheet name="tc074" sheetId="51" r:id="rId47"/>
+    <sheet name="tc047" sheetId="37" r:id="rId48"/>
+    <sheet name="tc046" sheetId="38" r:id="rId49"/>
+    <sheet name="tc004" sheetId="13" r:id="rId50"/>
+    <sheet name="tc019" sheetId="12" r:id="rId51"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -74,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="99">
   <si>
     <t>Project Name</t>
   </si>
@@ -365,6 +366,12 @@
   </si>
   <si>
     <t>delete notification Flow testing</t>
+  </si>
+  <si>
+    <t>New_module_name</t>
+  </si>
+  <si>
+    <t>Epic Mohit-creation module notification</t>
   </si>
 </sst>
 </file>
@@ -2640,9 +2647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3E5496-AF76-431E-B66C-9B684F671DD4}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
@@ -2697,6 +2702,31 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC692F0-41D1-4C10-B479-49A38BC3ED64}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294C6248-6B39-4869-9A5F-1A9888AB4466}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2739,7 +2769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5D97A-4287-4435-9AB2-0BB45EA4FBC3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2769,37 +2799,6 @@
       </c>
       <c r="C2" t="s">
         <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2850,6 +2849,37 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
   <dimension ref="A1:D2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TC-19 updated clickonMOdule() changed
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000DA4D5-7262-46E4-A9C3-C79ED4AF98E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B53830-0A57-41D8-916D-8B76B56D21F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="36" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="37" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -56,14 +56,14 @@
     <sheet name="tc053" sheetId="45" r:id="rId41"/>
     <sheet name="tc054" sheetId="46" r:id="rId42"/>
     <sheet name="tc055" sheetId="47" r:id="rId43"/>
-    <sheet name="tc063" sheetId="48" r:id="rId44"/>
-    <sheet name="tc064" sheetId="49" r:id="rId45"/>
-    <sheet name="tc073" sheetId="50" r:id="rId46"/>
-    <sheet name="tc074" sheetId="51" r:id="rId47"/>
-    <sheet name="tc047" sheetId="37" r:id="rId48"/>
-    <sheet name="tc046" sheetId="38" r:id="rId49"/>
-    <sheet name="tc004" sheetId="13" r:id="rId50"/>
-    <sheet name="tc019" sheetId="12" r:id="rId51"/>
+    <sheet name="tc047" sheetId="37" r:id="rId44"/>
+    <sheet name="tc046" sheetId="38" r:id="rId45"/>
+    <sheet name="tc004" sheetId="13" r:id="rId46"/>
+    <sheet name="tc019" sheetId="12" r:id="rId47"/>
+    <sheet name="tc065" sheetId="48" r:id="rId48"/>
+    <sheet name="tc066" sheetId="49" r:id="rId49"/>
+    <sheet name="tc077" sheetId="51" r:id="rId50"/>
+    <sheet name="tc073" sheetId="50" r:id="rId51"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="106">
   <si>
     <t>Project Name</t>
   </si>
@@ -341,44 +341,65 @@
     <t>RQ-437</t>
   </si>
   <si>
-    <t>STG- PulseCodeOnAzureCloude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Epic - update the module </t>
-  </si>
-  <si>
     <t>Hi, changing description</t>
   </si>
   <si>
     <t>Epic 13</t>
   </si>
   <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>Rqtitle</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t xml:space="preserve">type </t>
+  </si>
+  <si>
+    <t>Epic j17</t>
+  </si>
+  <si>
+    <t>RQ 123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description for requirement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should have </t>
+  </si>
+  <si>
+    <t>setModuleName</t>
+  </si>
+  <si>
+    <t>Module Testing (julie)</t>
+  </si>
+  <si>
+    <t>Module for testing</t>
+  </si>
+  <si>
     <t xml:space="preserve">Requirementitle </t>
   </si>
   <si>
-    <t>Notification for New Requirement 7-01-2026</t>
-  </si>
-  <si>
-    <t>Flow testing</t>
-  </si>
-  <si>
     <t>Notification for New Requirement 8-01-2026</t>
   </si>
   <si>
     <t>delete notification Flow testing</t>
   </si>
   <si>
-    <t>New_module_name</t>
-  </si>
-  <si>
-    <t>Epic Mohit-creation module notification</t>
+    <t>Epic - update the module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +435,13 @@
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -435,13 +463,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2344,15 +2373,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CEA2948-6B4B-43CF-AB32-61387B2A8875}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-  </cols>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -2523,210 +2546,6 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1567252D-CB85-4108-A7F9-F9A0823679CB}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="36.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA50CB24-998A-4723-A6C2-7AE3CF313CCB}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA3E5496-AF76-431E-B66C-9B684F671DD4}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="52.54296875" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDC692F0-41D1-4C10-B479-49A38BC3ED64}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{294C6248-6B39-4869-9A5F-1A9888AB4466}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2769,7 +2588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D5D97A-4287-4435-9AB2-0BB45EA4FBC3}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2799,6 +2618,182 @@
       </c>
       <c r="C2" t="s">
         <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="29.6328125" customWidth="1"/>
+    <col min="2" max="2" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3011021D-4819-4690-B3D7-76A026828EC9}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02E7FD6A-85B6-48DD-983C-2558ACC9E840}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2849,78 +2844,88 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6191B1E8-3F90-4D43-967E-7EE476AB5B81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{006ED08C-28C3-460C-941C-159F30186152}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47958D0E-DE08-4FC8-AE6D-9F22489AEEFF}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B43113-6F27-479A-A110-742EB7551220}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
-    <col min="3" max="3" width="22.54296875" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>91</v>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -3043,9 +3048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE237852-F036-4561-9C07-3E234A38E9FA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>

</xml_diff>

<commit_message>
TC-09 updated and updated method isRequirementVisible(String requirementId) in RequirementTabPage.java
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6AE50C-1CB8-426B-B526-9C4D414C4ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA076AA-913D-4B38-A27D-029954182900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="110">
   <si>
     <t>Project Name</t>
   </si>
@@ -957,45 +957,39 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:5">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1164,7 +1158,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B4C698C-6A33-4329-A05F-252C36050919}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TC-17 updated and data also updated
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EF00A6-2A17-4A1A-BCDC-1D9776805E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190EA6E1-E79B-4CCD-9DD5-323983BA1B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="111">
   <si>
     <t>Project Name</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Hi</t>
+  </si>
+  <si>
+    <t>Module 25</t>
   </si>
 </sst>
 </file>
@@ -959,7 +962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8911F113-D9E9-4D95-B104-6502D772C745}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1458,34 +1461,28 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:3">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TC-33 updated and data also updated
</commit_message>
<xml_diff>
--- a/testData/requirementTabTestData/requirementTab_testData.xlsx
+++ b/testData/requirementTabTestData/requirementTab_testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\requirementTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F9AF4D-22B8-46F5-977B-CB3456E15A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E442543-4B76-4DDF-940B-53B7BF4DF329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="18" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -1463,7 +1463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C4F00CF-C1AA-4EBC-984F-C64E09298E67}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1789,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C7D945-A188-4743-BACF-F57BC8D8AB86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>